<commit_message>
final testing files, expected analysis outcome files, final debugging
</commit_message>
<xml_diff>
--- a/Code/mdsc_deconvolution_simulation/Testing/Example set of parameters.xlsx
+++ b/Code/mdsc_deconvolution_simulation/Testing/Example set of parameters.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kuleuven-my.sharepoint.com/personal/tom_konings_kuleuven_be/Documents/Tom Konings/Software/DSC full app (git clone)/mDSC_apps/Code/mdsc_deconvolution_simulation/Testing/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="78" documentId="11_F25DC773A252ABDACC1048740918611A5BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3722613-D3DD-467B-9611-EF65EB5FCA52}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="645" yWindow="780" windowWidth="12810" windowHeight="7710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,91 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+  <si>
+    <t>Sampling rate (pts/s)</t>
+  </si>
+  <si>
+    <t>Starting temperature (°C)</t>
+  </si>
+  <si>
+    <t>Final temperature (°C)</t>
+  </si>
+  <si>
+    <t>Heating rate (°C/min)</t>
+  </si>
+  <si>
+    <t>Modulation amplitude (°c)</t>
+  </si>
+  <si>
+    <t>Modulation period (s)</t>
+  </si>
+  <si>
+    <t>Phase of the modulated heat flow with respect to the temperature modulation (rad)</t>
+  </si>
+  <si>
+    <t>Degree of smoothing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Gaussians </t>
+  </si>
+  <si>
+    <t>Slope of the reversing heat flow before the Tg (J/(g*°C))</t>
+  </si>
+  <si>
+    <t>Slope of the reversing heat flow after the Tg (J/(g*°C))</t>
+  </si>
+  <si>
+    <t>Starting value of the reversing heat flow (J/g)</t>
+  </si>
+  <si>
+    <t>Starting value of the total heat capacity (J/g)</t>
+  </si>
+  <si>
+    <t>THF Tg start, end, and midpoint separated by commas (°C)</t>
+  </si>
+  <si>
+    <t>RHF start, end, and midpoint separated by commas (°C)</t>
+  </si>
+  <si>
+    <t>Jump in heat capacity at the Tg (J/(g*°C))</t>
+  </si>
+  <si>
+    <t>Slope of the total heat capacity before the Tg (J/(g*°C))</t>
+  </si>
+  <si>
+    <t>Slope of the total heat capacity after the Tg (J/(g*°C))</t>
+  </si>
+  <si>
+    <t>70,90,80</t>
+  </si>
+  <si>
+    <t>Gaussian 1: Onset (°C), End (°C), Enthalpy (J/g)</t>
+  </si>
+  <si>
+    <t>Gaussian 2: Onset (°C), End (°C), Enthalpy (J/g)</t>
+  </si>
+  <si>
+    <t>Gaussian 3: Onset (°C), End (°C), Enthalpy (J/g)</t>
+  </si>
+  <si>
+    <t>100,120,1</t>
+  </si>
+  <si>
+    <t>140,160,-1.2</t>
+  </si>
+  <si>
+    <t>73,93,83</t>
+  </si>
+  <si>
+    <t>70,80,-0.3</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +419,189 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="77.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.21199999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>-1E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>-1.2E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>8.9999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>